<commit_message>
added RAG implementation and new updated data file
</commit_message>
<xml_diff>
--- a/Data Sample for Altro AI.xlsx
+++ b/Data Sample for Altro AI.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
   <si>
     <t>Project title</t>
   </si>
@@ -489,6 +489,9 @@
     </r>
   </si>
   <si>
+    <t>Locations</t>
+  </si>
+  <si>
     <t>Donation link</t>
   </si>
   <si>
@@ -498,16 +501,48 @@
 The Intent
 Our intent is to not only reduce the effect of violence that rattles cities around the world, but to go a step beyond – in creating a powerful and sustainable mechanism to initiate, establish and propagate peace via existing establishments of civic engagement, law enforcement and community groups.
 The Approach
-Our educational programs are based on scientifically proven breathing and meditation techniques that shift our perspective from merely ‘Reduction of Violence’ to ‘Actively Promoting Peace’. We work on creating a paradigm shift at the level of each individual, empowering them to become agents of change to collectively promote vibrant neighborhoods and peaceful and healthy cities.</t>
+Our educational programs are based on scientifically proven breathing and meditation techniques that shift our perspective from merely ‘Reduction of Violence’ to ‘Actively Promoting Peace’. We work on creating a paradigm shift at the level of each individual, empowering them to become agents of change to collectively promote vibrant neighborhoods and peaceful and healthy cities.
+Our Partners
+Cities4Peace invites city officials, law enforcement agencies and community organizations to #RethinkPeace in your city, and neighborhoods</t>
   </si>
   <si>
     <t>http://cities4peace.org/</t>
   </si>
   <si>
-    <t>USD 300</t>
-  </si>
-  <si>
     <t>https://iahv.networkforgood.com/projects/71211-cities-for-peace</t>
+  </si>
+  <si>
+    <t>About SKY Schools
+SKY Schools is dedicated to providing youth with a healthy body, a healthy mind and a healthy lifestyle. We do this by offering youth practical tools and life skills to manage stress and emotions. When students learn how to manage their stress in a healthy way, they exhibit greater confidence and motivation to succeed in school and make healthy choices when faced with life’s challenges.
+Young people face emotional issues such as low self-esteem, depression and anxiety that are a source of great stress, which inhibits learning. Without a healthy alternative, students often turn to unhealthy strategies to cope with these problems including: smoking, alcohol or drugs, aggression and violence, and withdrawal from social interaction. As students learn to reduce stress and manage emotions they gain the ability to focus and perform well academically at school, as well as the ability to build more positive relationships with their peers, parents and teachers.
+Healthy Body
+The Healthy Body module encourages physical fitness and healthy food choices through:
+Physical activity that includes exercise to stretch and strengthen the body
+Experiential processes that encourage mindful eating
+Interactive discussions on food and nutrition
+Healthy Mind
+The Healthy Mind module includes stress management and relaxation techniques that encourage a positive mental attitude through:
+Targeted breathing techniques that reduce stress, anger, anxiety and depression; improve focus and concentration; and enhance learning ability
+Relaxation exercises that encourage a calm state of mind
+Experiential processes that revitalize human values such as responsibility, respect, kindness, belonging, honesty, enthusiasm and service
+Healthy Lifestyle
+The Healthy Lifestyle module includes social-emotional learning and life skills in conflict resolution through:
+Teamwork exercises that teach how to manage emotions and resolve conflict
+Interactive processes that encourage pro-social behavior, problem solving and cooperation
+Dynamic discussions that teach goal setting and good decision-making
+Practical knowledge that increases self-confidence and inner-strength to help students handle peer pressure and make healthy choices when faced with life’s challenges</t>
+  </si>
+  <si>
+    <t>Georgia, Claifornia, North Carolina</t>
+  </si>
+  <si>
+    <t>https://yesforschools.networkforgood.com/projects/26485-generosity-108-support-yes-for-schools</t>
+  </si>
+  <si>
+    <t>USD 30000</t>
+  </si>
+  <si>
+    <t>https://iahv.networkforgood.com/projects/40449-iahv</t>
   </si>
   <si>
     <t>https://pmsh.iahv-peace.org/</t>
@@ -573,7 +608,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -615,8 +650,21 @@
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
       <sz val="15.0"/>
@@ -666,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -695,21 +743,30 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1442,9 +1499,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="50.25"/>
-    <col customWidth="1" min="2" max="2" width="58.25"/>
+    <col customWidth="1" min="2" max="2" width="595.5"/>
     <col customWidth="1" min="3" max="3" width="39.88"/>
-    <col customWidth="1" min="6" max="6" width="17.63"/>
+    <col customWidth="1" min="4" max="4" width="31.63"/>
+    <col customWidth="1" min="5" max="5" width="14.38"/>
+    <col customWidth="1" min="6" max="6" width="30.25"/>
+    <col customWidth="1" min="7" max="7" width="21.63"/>
     <col customWidth="1" min="8" max="8" width="72.75"/>
   </cols>
   <sheetData>
@@ -1458,8 +1518,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1471,24 +1531,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>93</v>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>21</v>
@@ -1496,58 +1556,104 @@
       <c r="G2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="H5" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E6" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>101</v>
+      <c r="G6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1558,11 +1664,15 @@
     <hyperlink r:id="rId4" ref="H3"/>
     <hyperlink r:id="rId5" ref="C4"/>
     <hyperlink r:id="rId6" ref="H4"/>
+    <hyperlink r:id="rId7" ref="C5"/>
+    <hyperlink r:id="rId8" ref="H5"/>
+    <hyperlink r:id="rId9" ref="C6"/>
+    <hyperlink r:id="rId10" ref="H6"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1581,55 +1691,55 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>103</v>
+      <c r="A1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>105</v>
+      <c r="A2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>106</v>
+      <c r="A3" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>107</v>
+      <c r="A4" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="14" t="s">
-        <v>108</v>
+      <c r="A5" s="17" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>110</v>
+      <c r="A6" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>112</v>
+      <c r="A8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>113</v>
+      <c r="A9" s="17" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>